<commit_message>
Organised main, finished Switch.xlsx
</commit_message>
<xml_diff>
--- a/Switchek.xlsx
+++ b/Switchek.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD94E485-D158-46E0-8EBC-F7DE3FB4BD9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Switch" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,14 +19,196 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Alhálózat</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Vlan</t>
+  </si>
+  <si>
+    <t>Eszköz</t>
+  </si>
+  <si>
+    <t>Fa0/1</t>
+  </si>
+  <si>
+    <t>Fa0/4</t>
+  </si>
+  <si>
+    <t>Fa0/5</t>
+  </si>
+  <si>
+    <t>Fa0/6</t>
+  </si>
+  <si>
+    <t>Fa0/20</t>
+  </si>
+  <si>
+    <t>Fa0/21</t>
+  </si>
+  <si>
+    <t>Fa0/22</t>
+  </si>
+  <si>
+    <t>Fa0/23</t>
+  </si>
+  <si>
+    <t>Fa0/24</t>
+  </si>
+  <si>
+    <t>Wireless Router0</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>IP Phone - mngt</t>
+  </si>
+  <si>
+    <t>Printer0</t>
+  </si>
+  <si>
+    <t>PC - mngt</t>
+  </si>
+  <si>
+    <t>IP Phone - backend</t>
+  </si>
+  <si>
+    <t>PC - backend</t>
+  </si>
+  <si>
+    <t>IP Phone - tester</t>
+  </si>
+  <si>
+    <t>PC - tester</t>
+  </si>
+  <si>
+    <t>Router</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>Fa0/7 - 0/19</t>
+  </si>
+  <si>
+    <t>IP Phone - frontend 1</t>
+  </si>
+  <si>
+    <t>PC - frontend 1</t>
+  </si>
+  <si>
+    <t>IP Phone - backend 1</t>
+  </si>
+  <si>
+    <t>PC - backend 1</t>
+  </si>
+  <si>
+    <t>IP Phone -UX 1</t>
+  </si>
+  <si>
+    <t>PC - UX 1</t>
+  </si>
+  <si>
+    <t>IP Phone - neteng 2</t>
+  </si>
+  <si>
+    <t>PC - neteng 2</t>
+  </si>
+  <si>
+    <t>IP Phone - tester 2</t>
+  </si>
+  <si>
+    <t>PC - tester 2</t>
+  </si>
+  <si>
+    <t>Fa0/3</t>
+  </si>
+  <si>
+    <t>Fa0/2</t>
+  </si>
+  <si>
+    <t>192.168.1.192/29</t>
+  </si>
+  <si>
+    <t>192.168.1.200/29</t>
+  </si>
+  <si>
+    <t>192.168.1.0/27</t>
+  </si>
+  <si>
+    <t>192.168.1.32/28</t>
+  </si>
+  <si>
+    <t>192.168.1.48/28</t>
+  </si>
+  <si>
+    <t>192.168.1.80/28</t>
+  </si>
+  <si>
+    <t>192.168.1.64/28</t>
+  </si>
+  <si>
+    <t>192.168.1.112/28</t>
+  </si>
+  <si>
+    <t>192.168.1.96/28</t>
+  </si>
+  <si>
+    <t>192.168.1.144/28</t>
+  </si>
+  <si>
+    <t>192.168.1.128/28</t>
+  </si>
+  <si>
+    <t>192.168.1.176/28</t>
+  </si>
+  <si>
+    <t>192.168.1.160/28</t>
+  </si>
+  <si>
+    <t>192.168.1.224/29</t>
+  </si>
+  <si>
+    <t>192.168.1.232/30</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -37,9 +220,126 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -49,11 +349,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +656,618 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2">
+        <v>31</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2">
+        <v>51</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2">
+        <v>50</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2">
+        <v>80</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2">
+        <v>90</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="3">
+        <v>21</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2">
+        <v>31</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2">
+        <v>30</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="2">
+        <v>61</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2">
+        <v>60</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2">
+        <v>80</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="2">
+        <v>100</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="3">
+        <v>21</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="2">
+        <v>20</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="2">
+        <v>41</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="2">
+        <v>40</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="2">
+        <v>51</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="2">
+        <v>50</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="2">
+        <v>80</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2">
+        <v>100</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>